<commit_message>
export initial Rating - Images
</commit_message>
<xml_diff>
--- a/InitialRating_Images.xlsx
+++ b/InitialRating_Images.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L122"/>
+  <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,13 +419,16 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2">
+        <v>19</v>
+      </c>
       <c r="L2">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="D3">
-        <v>1</v>
+      <c r="A3">
+        <v>20</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -433,48 +436,108 @@
       <c r="K3">
         <v>1</v>
       </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
-      <c r="K4">
-        <v>1</v>
+      <c r="A4">
+        <v>21</v>
       </c>
     </row>
     <row r="5">
-      <c r="L5">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
     </row>
     <row r="9">
+      <c r="A9">
+        <v>26</v>
+      </c>
       <c r="K9">
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>29</v>
+      </c>
+    </row>
     <row r="13">
+      <c r="A13">
+        <v>30</v>
+      </c>
       <c r="J13">
         <v>1</v>
       </c>
     </row>
     <row r="14">
+      <c r="A14">
+        <v>31</v>
+      </c>
       <c r="I14">
         <v>1</v>
       </c>
     </row>
     <row r="15">
+      <c r="A15">
+        <v>32</v>
+      </c>
       <c r="I15">
         <v>1</v>
       </c>
     </row>
     <row r="16">
+      <c r="A16">
+        <v>33</v>
+      </c>
       <c r="J16">
         <v>1</v>
       </c>
     </row>
     <row r="17">
+      <c r="A17">
+        <v>34</v>
+      </c>
       <c r="L17">
         <v>1</v>
       </c>
     </row>
     <row r="18">
+      <c r="A18">
+        <v>35</v>
+      </c>
       <c r="J18">
         <v>1</v>
       </c>
@@ -483,6 +546,9 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19">
+        <v>36</v>
+      </c>
       <c r="H19">
         <v>1</v>
       </c>
@@ -491,56 +557,94 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20">
+        <v>37</v>
+      </c>
       <c r="E20">
         <v>1</v>
       </c>
     </row>
     <row r="21">
+      <c r="A21">
+        <v>38</v>
+      </c>
       <c r="J21">
         <v>1</v>
       </c>
     </row>
     <row r="22">
+      <c r="A22">
+        <v>39</v>
+      </c>
       <c r="K22">
         <v>1</v>
       </c>
     </row>
     <row r="23">
+      <c r="A23">
+        <v>40</v>
+      </c>
       <c r="L23">
         <v>1</v>
       </c>
     </row>
     <row r="24">
+      <c r="A24">
+        <v>41</v>
+      </c>
       <c r="J24">
         <v>1</v>
       </c>
     </row>
     <row r="25">
+      <c r="A25">
+        <v>42</v>
+      </c>
       <c r="D25">
         <v>1</v>
       </c>
     </row>
     <row r="26">
+      <c r="A26">
+        <v>43</v>
+      </c>
       <c r="K26">
         <v>1</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27">
+        <v>44</v>
+      </c>
+    </row>
     <row r="28">
+      <c r="A28">
+        <v>45</v>
+      </c>
       <c r="L28">
         <v>1</v>
       </c>
     </row>
     <row r="29">
+      <c r="A29">
+        <v>46</v>
+      </c>
       <c r="J29">
         <v>1</v>
       </c>
     </row>
     <row r="30">
+      <c r="A30">
+        <v>47</v>
+      </c>
       <c r="L30">
         <v>1</v>
       </c>
     </row>
     <row r="31">
+      <c r="A31">
+        <v>48</v>
+      </c>
       <c r="I31">
         <v>1</v>
       </c>
@@ -549,31 +653,49 @@
       </c>
     </row>
     <row r="32">
+      <c r="A32">
+        <v>49</v>
+      </c>
       <c r="I32">
         <v>1</v>
       </c>
     </row>
     <row r="33">
+      <c r="A33">
+        <v>50</v>
+      </c>
       <c r="L33">
         <v>1</v>
       </c>
     </row>
     <row r="34">
+      <c r="A34">
+        <v>51</v>
+      </c>
       <c r="K34">
         <v>1</v>
       </c>
     </row>
     <row r="35">
+      <c r="A35">
+        <v>52</v>
+      </c>
       <c r="K35">
         <v>1</v>
       </c>
     </row>
     <row r="36">
+      <c r="A36">
+        <v>53</v>
+      </c>
       <c r="L36">
         <v>1</v>
       </c>
     </row>
     <row r="37">
+      <c r="A37">
+        <v>54</v>
+      </c>
       <c r="I37">
         <v>1</v>
       </c>
@@ -582,176 +704,301 @@
       </c>
     </row>
     <row r="38">
+      <c r="A38">
+        <v>55</v>
+      </c>
       <c r="L38">
         <v>1</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39">
+        <v>56</v>
+      </c>
+    </row>
     <row r="40">
+      <c r="A40">
+        <v>57</v>
+      </c>
       <c r="F40">
         <v>1</v>
       </c>
     </row>
     <row r="41">
+      <c r="A41">
+        <v>58</v>
+      </c>
       <c r="L41">
         <v>1</v>
       </c>
     </row>
     <row r="42">
+      <c r="A42">
+        <v>59</v>
+      </c>
       <c r="K42">
         <v>1</v>
       </c>
     </row>
     <row r="43">
+      <c r="A43">
+        <v>60</v>
+      </c>
       <c r="L43">
         <v>1</v>
       </c>
     </row>
     <row r="44">
+      <c r="A44">
+        <v>61</v>
+      </c>
       <c r="L44">
         <v>1</v>
       </c>
     </row>
     <row r="45">
+      <c r="A45">
+        <v>62</v>
+      </c>
       <c r="K45">
         <v>1</v>
       </c>
     </row>
     <row r="46">
+      <c r="A46">
+        <v>63</v>
+      </c>
       <c r="J46">
         <v>1</v>
       </c>
     </row>
     <row r="47">
+      <c r="A47">
+        <v>64</v>
+      </c>
       <c r="K47">
         <v>1</v>
       </c>
     </row>
     <row r="48">
+      <c r="A48">
+        <v>65</v>
+      </c>
       <c r="K48">
         <v>1</v>
       </c>
     </row>
     <row r="49">
+      <c r="A49">
+        <v>66</v>
+      </c>
       <c r="L49">
         <v>1</v>
       </c>
     </row>
     <row r="50">
+      <c r="A50">
+        <v>67</v>
+      </c>
       <c r="K50">
         <v>1</v>
       </c>
     </row>
     <row r="51">
+      <c r="A51">
+        <v>68</v>
+      </c>
       <c r="I51">
         <v>1</v>
       </c>
     </row>
     <row r="52">
+      <c r="A52">
+        <v>69</v>
+      </c>
       <c r="J52">
         <v>1</v>
       </c>
     </row>
     <row r="53">
+      <c r="A53">
+        <v>70</v>
+      </c>
       <c r="K53">
         <v>1</v>
       </c>
     </row>
     <row r="54">
+      <c r="A54">
+        <v>71</v>
+      </c>
       <c r="L54">
         <v>1</v>
       </c>
     </row>
     <row r="55">
+      <c r="A55">
+        <v>72</v>
+      </c>
       <c r="H55">
         <v>1</v>
       </c>
     </row>
     <row r="56">
+      <c r="A56">
+        <v>73</v>
+      </c>
       <c r="I56">
         <v>1</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57">
+        <v>74</v>
+      </c>
+    </row>
     <row r="58">
+      <c r="A58">
+        <v>75</v>
+      </c>
       <c r="G58">
         <v>1</v>
       </c>
     </row>
     <row r="59">
+      <c r="A59">
+        <v>76</v>
+      </c>
       <c r="L59">
         <v>1</v>
       </c>
     </row>
     <row r="60">
+      <c r="A60">
+        <v>77</v>
+      </c>
       <c r="E60">
         <v>1</v>
       </c>
     </row>
     <row r="61">
+      <c r="A61">
+        <v>78</v>
+      </c>
       <c r="F61">
         <v>1</v>
       </c>
     </row>
     <row r="62">
+      <c r="A62">
+        <v>79</v>
+      </c>
       <c r="K62">
         <v>1</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63">
+        <v>80</v>
+      </c>
+    </row>
     <row r="64">
+      <c r="A64">
+        <v>81</v>
+      </c>
       <c r="L64">
         <v>1</v>
       </c>
     </row>
     <row r="65">
+      <c r="A65">
+        <v>82</v>
+      </c>
       <c r="L65">
         <v>1</v>
       </c>
     </row>
     <row r="66">
+      <c r="A66">
+        <v>83</v>
+      </c>
       <c r="L66">
         <v>1</v>
       </c>
     </row>
     <row r="67">
+      <c r="A67">
+        <v>84</v>
+      </c>
       <c r="E67">
         <v>1</v>
       </c>
     </row>
     <row r="68">
+      <c r="A68">
+        <v>85</v>
+      </c>
       <c r="J68">
         <v>1</v>
       </c>
     </row>
     <row r="69">
+      <c r="A69">
+        <v>86</v>
+      </c>
       <c r="G69">
         <v>1</v>
       </c>
     </row>
     <row r="70">
+      <c r="A70">
+        <v>87</v>
+      </c>
       <c r="H70">
         <v>1</v>
       </c>
     </row>
     <row r="71">
+      <c r="A71">
+        <v>88</v>
+      </c>
       <c r="K71">
         <v>1</v>
       </c>
     </row>
     <row r="72">
+      <c r="A72">
+        <v>89</v>
+      </c>
       <c r="I72">
         <v>1</v>
       </c>
     </row>
     <row r="73">
+      <c r="A73">
+        <v>90</v>
+      </c>
       <c r="I73">
         <v>1</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74">
+        <v>91</v>
+      </c>
+    </row>
     <row r="75">
+      <c r="A75">
+        <v>92</v>
+      </c>
       <c r="I75">
         <v>1</v>
       </c>
     </row>
     <row r="76">
+      <c r="A76">
+        <v>93</v>
+      </c>
       <c r="I76">
         <v>1</v>
       </c>
@@ -760,56 +1007,99 @@
       </c>
     </row>
     <row r="77">
+      <c r="A77">
+        <v>94</v>
+      </c>
       <c r="H77">
         <v>1</v>
       </c>
     </row>
     <row r="78">
+      <c r="A78">
+        <v>95</v>
+      </c>
       <c r="J78">
         <v>1</v>
       </c>
     </row>
     <row r="79">
+      <c r="A79">
+        <v>96</v>
+      </c>
       <c r="I79">
         <v>1</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80">
+        <v>97</v>
+      </c>
+    </row>
     <row r="81">
+      <c r="A81">
+        <v>98</v>
+      </c>
       <c r="K81">
         <v>1</v>
       </c>
     </row>
     <row r="82">
+      <c r="A82">
+        <v>99</v>
+      </c>
       <c r="L82">
         <v>1</v>
       </c>
     </row>
     <row r="83">
+      <c r="A83">
+        <v>100</v>
+      </c>
       <c r="H83">
         <v>1</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84">
+        <v>101</v>
+      </c>
+    </row>
     <row r="85">
+      <c r="A85">
+        <v>102</v>
+      </c>
       <c r="J85">
         <v>1</v>
       </c>
     </row>
     <row r="86">
+      <c r="A86">
+        <v>103</v>
+      </c>
       <c r="G86">
         <v>1</v>
       </c>
     </row>
     <row r="87">
+      <c r="A87">
+        <v>104</v>
+      </c>
       <c r="K87">
         <v>1</v>
       </c>
     </row>
     <row r="88">
+      <c r="A88">
+        <v>105</v>
+      </c>
       <c r="H88">
         <v>1</v>
       </c>
     </row>
     <row r="89">
+      <c r="A89">
+        <v>106</v>
+      </c>
       <c r="J89">
         <v>1</v>
       </c>
@@ -818,26 +1108,51 @@
       </c>
     </row>
     <row r="90">
+      <c r="A90">
+        <v>107</v>
+      </c>
       <c r="G90">
         <v>1</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91">
+        <v>108</v>
+      </c>
+    </row>
     <row r="92">
+      <c r="A92">
+        <v>109</v>
+      </c>
       <c r="I92">
         <v>1</v>
       </c>
     </row>
     <row r="93">
+      <c r="A93">
+        <v>110</v>
+      </c>
       <c r="K93">
         <v>1</v>
       </c>
     </row>
     <row r="94">
+      <c r="A94">
+        <v>111</v>
+      </c>
       <c r="K94">
         <v>1</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95">
+        <v>112</v>
+      </c>
+    </row>
     <row r="96">
+      <c r="A96">
+        <v>113</v>
+      </c>
       <c r="I96">
         <v>1</v>
       </c>
@@ -845,114 +1160,210 @@
         <v>2</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97">
+        <v>114</v>
+      </c>
+    </row>
     <row r="98">
+      <c r="A98">
+        <v>115</v>
+      </c>
       <c r="H98">
         <v>1</v>
       </c>
     </row>
     <row r="99">
+      <c r="A99">
+        <v>116</v>
+      </c>
       <c r="J99">
         <v>1</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100">
+        <v>117</v>
+      </c>
+    </row>
     <row r="101">
+      <c r="A101">
+        <v>118</v>
+      </c>
       <c r="K101">
         <v>1</v>
       </c>
     </row>
     <row r="102">
+      <c r="A102">
+        <v>119</v>
+      </c>
       <c r="K102">
         <v>1</v>
       </c>
     </row>
     <row r="103">
+      <c r="A103">
+        <v>120</v>
+      </c>
       <c r="L103">
         <v>1</v>
       </c>
     </row>
     <row r="104">
+      <c r="A104">
+        <v>121</v>
+      </c>
       <c r="L104">
         <v>1</v>
       </c>
     </row>
     <row r="105">
+      <c r="A105">
+        <v>122</v>
+      </c>
       <c r="J105">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="K105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>123</v>
       </c>
     </row>
     <row r="107">
+      <c r="A107">
+        <v>124</v>
+      </c>
       <c r="H107">
         <v>1</v>
       </c>
     </row>
+    <row r="108">
+      <c r="A108">
+        <v>125</v>
+      </c>
+    </row>
     <row r="109">
+      <c r="A109">
+        <v>126</v>
+      </c>
       <c r="J109">
         <v>1</v>
       </c>
     </row>
     <row r="110">
+      <c r="A110">
+        <v>127</v>
+      </c>
       <c r="L110">
         <v>1</v>
       </c>
     </row>
     <row r="111">
+      <c r="A111">
+        <v>128</v>
+      </c>
       <c r="H111">
         <v>1</v>
       </c>
     </row>
     <row r="112">
+      <c r="A112">
+        <v>129</v>
+      </c>
       <c r="J112">
         <v>1</v>
       </c>
     </row>
     <row r="113">
+      <c r="A113">
+        <v>130</v>
+      </c>
       <c r="L113">
         <v>1</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114">
+        <v>131</v>
+      </c>
+    </row>
     <row r="115">
+      <c r="A115">
+        <v>132</v>
+      </c>
       <c r="L115">
         <v>1</v>
       </c>
     </row>
     <row r="116">
+      <c r="A116">
+        <v>133</v>
+      </c>
       <c r="C116">
         <v>1</v>
       </c>
     </row>
     <row r="117">
+      <c r="A117">
+        <v>134</v>
+      </c>
       <c r="K117">
         <v>1</v>
       </c>
     </row>
     <row r="118">
+      <c r="A118">
+        <v>135</v>
+      </c>
       <c r="K118">
         <v>1</v>
       </c>
     </row>
     <row r="119">
+      <c r="A119">
+        <v>136</v>
+      </c>
       <c r="K119">
         <v>1</v>
       </c>
     </row>
     <row r="120">
+      <c r="A120">
+        <v>137</v>
+      </c>
       <c r="K120">
         <v>1</v>
       </c>
     </row>
     <row r="121">
+      <c r="A121">
+        <v>138</v>
+      </c>
       <c r="L121">
         <v>1</v>
       </c>
     </row>
     <row r="122">
+      <c r="A122">
+        <v>139</v>
+      </c>
       <c r="K122">
         <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L122"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L123"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>